<commit_message>
deploy telegram bot to heroku
</commit_message>
<xml_diff>
--- a/TelegramBot/report_30_days.xlsx
+++ b/TelegramBot/report_30_days.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,93 +356,187 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Дата и время измерения</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Систолическое</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Диасталическое</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>10</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2020-04-03 02:10</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>10</v>
       </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>10</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2020-04-03 02:10</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>10</v>
       </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2020-04-03 03:47:39</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>110</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2020-04-03 06:47:07</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>80</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2020-04-10 09:44:47</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>111</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2020-04-10 10:18:12</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>181</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>91</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2020-04-10 13:18:07</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>110</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2020-04-10 13:18:11</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>80</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2020-04-10 13:20:24</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>120</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>85</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2020-04-10 13:20:31</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>110</v>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>76</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2020-04-10 13:30:42</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>177</v>
+      </c>
+      <c r="C12" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2020-04-10 13:43:14</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>110</v>
+      </c>
+      <c r="C13" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2020-04-14 00:22:19</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>114</v>
+      </c>
+      <c r="C14" t="n">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>